<commit_message>
agrego excel de pruebas
</commit_message>
<xml_diff>
--- a/Pruebas Proyecto Python Hollmann.xlsx
+++ b/Pruebas Proyecto Python Hollmann.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28103"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DD01EB2-18B7-45E7-BFA4-F578A4A6C630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F12360A-3AA0-48E7-8449-7FFDC7782210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BCD56C2B-7EFC-4439-B006-08DEE2259B23}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -117,12 +117,6 @@
   </si>
   <si>
     <t>Todos van a una página o sección distinta</t>
-  </si>
-  <si>
-    <t>Carga de productos</t>
-  </si>
-  <si>
-    <t>Nuevo instrumento visible dependiendo de la categoria del instrumento (ejemplo:guitarra). Una vez el instrumento es ingresado a la BD el usuario es dirigido al inicio (El ingreso del instrumento musical se realiza en el formulario disponible en el inicio de la página web</t>
   </si>
   <si>
     <t>Carga de Comentario</t>
@@ -293,11 +287,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524B7CD3-7E22-4FB7-BD6C-740AE7574A93}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -633,65 +627,65 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
@@ -773,7 +767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="121.5">
+    <row r="10" spans="1:6" ht="30.75">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -793,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30.75">
+    <row r="11" spans="1:6" ht="91.5">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -803,11 +797,11 @@
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>30</v>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>23</v>
@@ -821,19 +815,19 @@
         <v>45540</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="121.5">
+    <row r="13" spans="1:6" ht="30.75">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -853,7 +847,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30.75">
+    <row r="14" spans="1:6" ht="60.75">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -870,26 +864,6 @@
         <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="60.75">
-      <c r="A15" s="3">
-        <v>9</v>
-      </c>
-      <c r="B15" s="4">
-        <v>45540</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>